<commit_message>
Updated Medicaid load scripts for FY22
and started on QA
</commit_message>
<xml_diff>
--- a/greenplum/datawarehouse/QA/medicaid/dw_staging/outputs/dw-enrollment-qa.xlsx
+++ b/greenplum/datawarehouse/QA/medicaid/dw_staging/outputs/dw-enrollment-qa.xlsx
@@ -17,7 +17,7 @@
     <t xml:space="preserve">Data Warehouse Enrollment Tables QA</t>
   </si>
   <si>
-    <t xml:space="preserve">Run date: 2022-10-26</t>
+    <t xml:space="preserve">Run date: 2023-09-11</t>
   </si>
   <si>
     <t xml:space="preserve">source_list</t>
@@ -32,22 +32,22 @@
     <t xml:space="preserve">Data_warehouse Monthly Enrollment Table</t>
   </si>
   <si>
-    <t xml:space="preserve">13029774</t>
-  </si>
-  <si>
-    <t xml:space="preserve">586823622</t>
+    <t xml:space="preserve">10126890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">436459081</t>
   </si>
   <si>
     <t xml:space="preserve">Data_warehouse Yearly Enrollment Table</t>
   </si>
   <si>
+    <t xml:space="preserve">Data_warehouse Fiscal Yearly Enrollment Table</t>
+  </si>
+  <si>
     <t xml:space="preserve">TACC server medicaid schema</t>
   </si>
   <si>
     <t xml:space="preserve">SPC server medicaid schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">586823632</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="39.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="45.71" hidden="0" customWidth="1"/>
     <col min="2" max="2" width="16.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="15.71" hidden="0" customWidth="1"/>
   </cols>
@@ -446,7 +446,18 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>